<commit_message>
Users can now elect to ignore modules in their report that are only dev dependencies
</commit_message>
<xml_diff>
--- a/license-details.xlsx
+++ b/license-details.xlsx
@@ -701,7 +701,7 @@
         <v>https://github.com/isaacs/inherits#readme</v>
       </c>
       <c r="G16" t="str">
-        <v/>
+        <v>isaacs</v>
       </c>
     </row>
     <row r="17">
@@ -913,7 +913,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -941,9 +941,129 @@
         <v>Author</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>should/13.2.3</v>
+      </c>
+      <c r="C2" t="str">
+        <v>test framework agnostic BDD-style assertions</v>
+      </c>
+      <c r="D2" t="str">
+        <v>MIT</v>
+      </c>
+      <c r="F2" t="str">
+        <v>https://github.com/shouldjs/should.js</v>
+      </c>
+      <c r="G2" t="str">
+        <v>TJ Holowaychuk</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>should-equal/2.0.0</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Deep comparison of 2 instances for should.js</v>
+      </c>
+      <c r="D3" t="str">
+        <v>MIT</v>
+      </c>
+      <c r="F3" t="str">
+        <v>https://github.com/shouldjs/equal</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Denis Bardadym</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>should-format/3.0.3</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Formatting of objects for should.js</v>
+      </c>
+      <c r="D4" t="str">
+        <v>MIT</v>
+      </c>
+      <c r="F4" t="str">
+        <v>https://github.com/shouldjs/format#readme</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Denis Bardadym</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>should-type/1.4.0</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Simple module to get instance type. Like a bit more advanced version of typeof</v>
+      </c>
+      <c r="D5" t="str">
+        <v>MIT</v>
+      </c>
+      <c r="F5" t="str">
+        <v>https://github.com/shouldjs/type</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Denis Bardadym</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>should-type-adaptors/1.1.0</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Small utility functions to use the same traversing etc code on different types</v>
+      </c>
+      <c r="D6" t="str">
+        <v>MIT</v>
+      </c>
+      <c r="F6" t="str">
+        <v>https://github.com/shouldjs/type-adaptors#readme</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Denis Bardadym</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>should-util/1.0.0</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Utility functions</v>
+      </c>
+      <c r="D7" t="str">
+        <v>MIT</v>
+      </c>
+      <c r="F7" t="str">
+        <v>https://github.com/shouldjs/util#readme</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Denis Bardadym</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correcting minor issue with error message when no valid config defined.
</commit_message>
<xml_diff>
--- a/license-details.xlsx
+++ b/license-details.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -769,19 +769,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="str">
-        <v>once/1.4.0</v>
+        <v>moment/2.22.2</v>
       </c>
       <c r="C20" t="str">
-        <v>Run a function exactly one time</v>
+        <v>Parse, validate, manipulate, and display dates</v>
       </c>
       <c r="D20" t="str">
-        <v>ISC</v>
+        <v>MIT</v>
       </c>
       <c r="F20" t="str">
-        <v>https://github.com/isaacs/once#readme</v>
+        <v>http://momentjs.com</v>
       </c>
       <c r="G20" t="str">
-        <v>Isaac Z. Schlueter</v>
+        <v>Iskren Ivov Chernev</v>
       </c>
     </row>
     <row r="21">
@@ -789,19 +789,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="str">
-        <v>path-is-absolute/1.0.1</v>
+        <v>once/1.4.0</v>
       </c>
       <c r="C21" t="str">
-        <v>Node.js 0.12 path.isAbsolute() ponyfill</v>
+        <v>Run a function exactly one time</v>
       </c>
       <c r="D21" t="str">
-        <v>MIT</v>
+        <v>ISC</v>
       </c>
       <c r="F21" t="str">
-        <v>https://github.com/sindresorhus/path-is-absolute#readme</v>
+        <v>https://github.com/isaacs/once#readme</v>
       </c>
       <c r="G21" t="str">
-        <v>Sindre Sorhus</v>
+        <v>Isaac Z. Schlueter</v>
       </c>
     </row>
     <row r="22">
@@ -809,19 +809,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="str">
-        <v>printj/1.1.2</v>
+        <v>path-is-absolute/1.0.1</v>
       </c>
       <c r="C22" t="str">
-        <v>Pure-JS printf</v>
+        <v>Node.js 0.12 path.isAbsolute() ponyfill</v>
       </c>
       <c r="D22" t="str">
-        <v>Apache-2.0</v>
+        <v>MIT</v>
       </c>
       <c r="F22" t="str">
-        <v>http://sheetjs.com/opensource</v>
+        <v>https://github.com/sindresorhus/path-is-absolute#readme</v>
       </c>
       <c r="G22" t="str">
-        <v>sheetjs</v>
+        <v>Sindre Sorhus</v>
       </c>
     </row>
     <row r="23">
@@ -829,10 +829,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="str">
-        <v>ssf/0.10.2</v>
+        <v>printj/1.1.2</v>
       </c>
       <c r="C23" t="str">
-        <v>Format data using ECMA-376 spreadsheet Format Codes</v>
+        <v>Pure-JS printf</v>
       </c>
       <c r="D23" t="str">
         <v>Apache-2.0</v>
@@ -849,19 +849,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="str">
-        <v>wrappy/1.0.2</v>
+        <v>ssf/0.10.2</v>
       </c>
       <c r="C24" t="str">
-        <v>Callback wrapping utility</v>
+        <v>Format data using ECMA-376 spreadsheet Format Codes</v>
       </c>
       <c r="D24" t="str">
-        <v>ISC</v>
+        <v>Apache-2.0</v>
       </c>
       <c r="F24" t="str">
-        <v>https://github.com/npm/wrappy</v>
+        <v>http://sheetjs.com/opensource</v>
       </c>
       <c r="G24" t="str">
-        <v>Isaac Z. Schlueter</v>
+        <v>sheetjs</v>
       </c>
     </row>
     <row r="25">
@@ -869,19 +869,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="str">
-        <v>xlsx/0.13.2</v>
+        <v>wrappy/1.0.2</v>
       </c>
       <c r="C25" t="str">
-        <v>SheetJS Spreadsheet data parser and writer</v>
+        <v>Callback wrapping utility</v>
       </c>
       <c r="D25" t="str">
-        <v>Apache-2.0</v>
+        <v>ISC</v>
       </c>
       <c r="F25" t="str">
-        <v>http://sheetjs.com/opensource</v>
+        <v>https://github.com/npm/wrappy</v>
       </c>
       <c r="G25" t="str">
-        <v>sheetjs</v>
+        <v>Isaac Z. Schlueter</v>
       </c>
     </row>
     <row r="26">
@@ -889,24 +889,44 @@
         <v>25</v>
       </c>
       <c r="B26" t="str">
+        <v>xlsx/0.13.2</v>
+      </c>
+      <c r="C26" t="str">
+        <v>SheetJS Spreadsheet data parser and writer</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Apache-2.0</v>
+      </c>
+      <c r="F26" t="str">
+        <v>http://sheetjs.com/opensource</v>
+      </c>
+      <c r="G26" t="str">
+        <v>sheetjs</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="str">
         <v>xregexp/4.2.0</v>
       </c>
-      <c r="C26" t="str">
+      <c r="C27" t="str">
         <v>Extended regular expressions</v>
       </c>
-      <c r="D26" t="str">
-        <v>MIT</v>
-      </c>
-      <c r="F26" t="str">
+      <c r="D27" t="str">
+        <v>MIT</v>
+      </c>
+      <c r="F27" t="str">
         <v>http://xregexp.com/</v>
       </c>
-      <c r="G26" t="str">
+      <c r="G27" t="str">
         <v>Steven Levithan</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G26"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G27"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>